<commit_message>
Fc layer experiments results
Former-commit-id: 53aefab53c5137e9235c44af034280ea22439580
Former-commit-id: c2f9f9821c8abfaadefed7595736f73dea20810d [formerly e35c2cebd4952a3f3d63e252cb6ae87e067acd03]
Former-commit-id: 09639cb8a54831a0d6b74dba25db6508e64f3acd
</commit_message>
<xml_diff>
--- a/side_effects/rapport/fc-output.xlsx
+++ b/side_effects/rapport/fc-output.xlsx
@@ -380,7 +380,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -402,13 +402,13 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.1107722917514288</v>
+        <v>0.6090525509482942</v>
       </c>
       <c r="C2">
-        <v>0.5924634926288258</v>
+        <v>0.9777443151841506</v>
       </c>
       <c r="D2">
-        <v>200</v>
+        <v>150</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -416,13 +416,13 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>0.1280943337875468</v>
+        <v>0.6158446575419874</v>
       </c>
       <c r="C3">
-        <v>0.6117532985828138</v>
+        <v>0.9781730676537722</v>
       </c>
       <c r="D3">
-        <v>350</v>
+        <v>450</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -430,13 +430,13 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.03419361072887989</v>
+        <v>0.5924273823341631</v>
       </c>
       <c r="C4">
-        <v>0.5292044184047869</v>
+        <v>0.9785545357999735</v>
       </c>
       <c r="D4">
-        <v>300</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -444,13 +444,13 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.1510282802398129</v>
+        <v>0.6174638305355407</v>
       </c>
       <c r="C5">
-        <v>0.6172141256946724</v>
+        <v>0.9790965634947779</v>
       </c>
       <c r="D5">
-        <v>25</v>
+        <v>350</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -458,13 +458,13 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.1001968031505989</v>
+        <v>0.603532451203402</v>
       </c>
       <c r="C6">
-        <v>0.590659945383867</v>
+        <v>0.9777717296365427</v>
       </c>
       <c r="D6">
-        <v>250</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -472,13 +472,13 @@
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.04271122048783672</v>
+        <v>0.6077908466471653</v>
       </c>
       <c r="C7">
-        <v>0.6003084219292231</v>
+        <v>0.9786448284056865</v>
       </c>
       <c r="D7">
-        <v>400</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -486,13 +486,13 @@
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.1098315301599631</v>
+        <v>0.5920415103264995</v>
       </c>
       <c r="C8">
-        <v>0.6026354870757277</v>
+        <v>0.9777780505941711</v>
       </c>
       <c r="D8">
-        <v>450</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -500,13 +500,13 @@
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.1172609294686825</v>
+        <v>0.6208749301584144</v>
       </c>
       <c r="C9">
-        <v>0.600741129334521</v>
+        <v>0.9798951672870251</v>
       </c>
       <c r="D9">
-        <v>500</v>
+        <v>512</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -514,13 +514,97 @@
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.07741946646914136</v>
+        <v>0.6254428465434397</v>
       </c>
       <c r="C10">
-        <v>0.5610375835144352</v>
+        <v>0.9801289712231603</v>
       </c>
       <c r="D10">
-        <v>150</v>
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>0.6092459848759443</v>
+      </c>
+      <c r="C11">
+        <v>0.9780775366505514</v>
+      </c>
+      <c r="D11">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>0.6085730073322152</v>
+      </c>
+      <c r="C12">
+        <v>0.9767224112683015</v>
+      </c>
+      <c r="D12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>0.6221821314463949</v>
+      </c>
+      <c r="C13">
+        <v>0.9783465401317034</v>
+      </c>
+      <c r="D13">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>0.6057427544415619</v>
+      </c>
+      <c r="C14">
+        <v>0.9781840931880694</v>
+      </c>
+      <c r="D14">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.5967852939947144</v>
+      </c>
+      <c r="C15">
+        <v>0.9773693057641633</v>
+      </c>
+      <c r="D15">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>0.5952083146592653</v>
+      </c>
+      <c r="C16">
+        <v>0.9776092170085141</v>
+      </c>
+      <c r="D16">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>